<commit_message>
adjust problem 5 - cont -> simple
</commit_message>
<xml_diff>
--- a/Homework/HW4/problem5.xlsx
+++ b/Homework/HW4/problem5.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="FLOATING" sheetId="1" r:id="rId1"/>
@@ -738,19 +738,19 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="5">
-        <f>(EXP($C$2 * 1) - (1 / A23)) / (A23 - (1 / A23))</f>
-        <v>0.38718397874376587</v>
+        <f>(1 + $C$2 - (1 / A23)) / (A23 - (1 / A23))</f>
+        <v>0.38713584255482014</v>
       </c>
       <c r="B31" s="5">
-        <f>(EXP($C$2 * 1) - (1 / B23)) / (B23 - (1 / B23))</f>
-        <v>0.41644587282361439</v>
+        <f>(1 + $C$2 - (1 / B23)) / (B23 - (1 / B23))</f>
+        <v>0.41638305659064107</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="5"/>
       <c r="B32" s="5">
-        <f>(EXP($C$2 * 1) - (1 / B24)) / (B24 - (1 / B24))</f>
-        <v>0.35210586743335492</v>
+        <f>(1 + $C$2 - (1 / B24)) / (B24 - (1 / B24))</f>
+        <v>0.35206935757615671</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -772,11 +772,11 @@
     <row r="36" spans="1:3">
       <c r="A36" s="4">
         <f>(A31 * B36 + (1 - A31) *B38) / (1 + $C$2)</f>
-        <v>5.6958268635506277</v>
+        <v>5.6945549641692308</v>
       </c>
       <c r="B36" s="4">
         <f>(B31 * C36 + (1 - B31) *C37) / (1 + $C$2)</f>
-        <v>13.174083068235372</v>
+        <v>13.172445215982766</v>
       </c>
       <c r="C36" s="4">
         <f>MAX(C6 - $D$2, 0)</f>
@@ -795,7 +795,7 @@
       <c r="A38" s="4"/>
       <c r="B38" s="4">
         <f>(B32 * C38 + (1 - B32) *C39) / (1 + $C$2)</f>
-        <v>1.063926547137823</v>
+        <v>1.0638162285947421</v>
       </c>
       <c r="C38" s="4">
         <f>MAX(C8 - $D$2, 0)</f>

</xml_diff>